<commit_message>
Now working again if you put libraries in global.R
</commit_message>
<xml_diff>
--- a/Köpa eller hyra_1.xlsx
+++ b/Köpa eller hyra_1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claesbackman/Dropbox/Public Lectures/Course material/Verktyg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au641277\Documents\GitHub\Verktyg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25460F2-2704-8D4C-9AC8-5555FFD84C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25515" windowHeight="14475"/>
   </bookViews>
   <sheets>
     <sheet name="Alla år" sheetId="1" r:id="rId1"/>
@@ -44,7 +43,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">398339</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -374,7 +373,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
@@ -386,10 +385,10 @@
     <numFmt numFmtId="170" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -563,7 +562,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -639,6 +638,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,23 +667,13 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -984,37 +984,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L120"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="102" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.83203125" customWidth="1"/>
+    <col min="7" max="7" width="75.875" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="71"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="80"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>61</v>
       </c>
@@ -1022,11 +1022,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>3061.1160154725289</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1109,13 +1109,13 @@
         <v>3061.1160154725289</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="71"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="80"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>162435</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>65</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>402220.39764592354</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>522220.39764592354</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1227,23 +1227,23 @@
       </c>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="G18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+    <row r="19" spans="1:9">
+      <c r="A19" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="80"/>
       <c r="F19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1261,11 +1261,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="86">
         <v>2.0000001E-2</v>
       </c>
       <c r="C21">
@@ -1282,11 +1282,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="87">
         <v>0.02</v>
       </c>
       <c r="C22">
@@ -1300,7 +1300,7 @@
         <v>46227.972674024626</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>46227.972674024626</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>4.47E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1335,17 +1335,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="B26" s="4"/>
       <c r="F26" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="71" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="71"/>
+      <c r="B27" s="80"/>
       <c r="F27" t="s">
         <v>43</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1422,16 +1422,16 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="F33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="77">
+      <c r="G33" s="71">
         <f>G28+G29+G30</f>
         <v>440254.77588841517</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
@@ -1446,21 +1446,24 @@
         <v>-3061.1160154725289</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="18">
       <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="86">
-        <f>(G37-B110)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
+      <c r="B35" s="79">
+        <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
         <v>3061.1160154725289</v>
       </c>
-      <c r="C35" s="69"/>
+      <c r="C35" s="69">
+        <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
+        <v>3061.1160154725289</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>58</v>
       </c>
       <c r="G35" s="49"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1479,49 +1482,49 @@
       <c r="F37" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="78">
+      <c r="G37" s="72">
         <f>G9+G16+G23-G33</f>
         <v>568448.40629108495</v>
       </c>
-      <c r="H37" s="78">
+      <c r="H37" s="72">
         <f>H9+H16+H22+H31+H34</f>
         <v>568448.37031994818</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
+    <row r="39" spans="1:12" ht="16.5" thickBot="1">
+      <c r="A39" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="76"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="43"/>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="75"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="83"/>
+      <c r="K40" s="84"/>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="51"/>
       <c r="B41" s="52">
         <v>1</v>
@@ -1554,7 +1557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="16.5" thickBot="1">
       <c r="A42" s="51" t="s">
         <v>24</v>
       </c>
@@ -1599,7 +1602,7 @@
       </c>
       <c r="L42" s="64"/>
     </row>
-    <row r="43" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" s="11" customFormat="1">
       <c r="A43" s="32" t="s">
         <v>37</v>
       </c>
@@ -1614,7 +1617,7 @@
       <c r="J43" s="33"/>
       <c r="K43" s="34"/>
     </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="11" customFormat="1">
       <c r="A44" s="35" t="s">
         <v>28</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="11" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>697000</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="11" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="35"/>
       <c r="B46" s="38"/>
       <c r="C46" s="39"/>
@@ -1717,7 +1720,7 @@
       <c r="J46" s="39"/>
       <c r="K46" s="40"/>
     </row>
-    <row r="47" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="11" customFormat="1">
       <c r="A47" s="35" t="s">
         <v>30</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="11" customFormat="1">
       <c r="A48" s="35" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>1343916.379344122</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="11" customFormat="1">
       <c r="A49" s="57" t="s">
         <v>38</v>
       </c>
@@ -1822,7 +1825,7 @@
       <c r="J49" s="19"/>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" s="11" customFormat="1">
       <c r="A50" s="21" t="s">
         <v>22</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>14636.999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" s="11" customFormat="1">
       <c r="A51" s="23" t="s">
         <v>32</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" s="11" customFormat="1">
       <c r="A52" s="23" t="s">
         <v>20</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" s="11" customFormat="1">
       <c r="A53" s="23" t="s">
         <v>21</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" s="11" customFormat="1">
       <c r="A54" s="23"/>
       <c r="B54" s="19">
         <f>SUM(B50:B53)</f>
@@ -2045,7 +2048,7 @@
         <v>72637</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" s="11" customFormat="1">
       <c r="A55" s="58" t="s">
         <v>39</v>
       </c>
@@ -2060,7 +2063,7 @@
       <c r="J55" s="25"/>
       <c r="K55" s="59"/>
     </row>
-    <row r="56" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" s="11" customFormat="1">
       <c r="A56" s="60" t="s">
         <v>9</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" s="11" customFormat="1">
       <c r="A57" s="60" t="s">
         <v>14</v>
       </c>
@@ -2100,7 +2103,7 @@
         <v>-150000</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" s="11" customFormat="1">
       <c r="A58" s="62" t="s">
         <v>26</v>
       </c>
@@ -2115,7 +2118,7 @@
       <c r="J58" s="54"/>
       <c r="K58" s="28"/>
     </row>
-    <row r="59" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" s="11" customFormat="1">
       <c r="A59" s="26" t="s">
         <v>51</v>
       </c>
@@ -2124,44 +2127,44 @@
         <v>153000</v>
       </c>
       <c r="C59" s="27">
-        <f>(B59-B62)*(1+$B$22)</f>
+        <f t="shared" ref="C59:K59" si="10">(B59-B62)*(1+$B$22)</f>
         <v>156060</v>
       </c>
       <c r="D59" s="27">
-        <f>(C59-C62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>159181.20000000001</v>
       </c>
       <c r="E59" s="27">
-        <f>(D59-D62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>162364.82400000002</v>
       </c>
       <c r="F59" s="27">
-        <f>(E59-E62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>165612.12048000001</v>
       </c>
       <c r="G59" s="27">
-        <f>(F59-F62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>168924.36288960002</v>
       </c>
       <c r="H59" s="27">
-        <f>(G59-G62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>172302.85014739202</v>
       </c>
       <c r="I59" s="27">
-        <f>(H59-H62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>175748.90715033986</v>
       </c>
       <c r="J59" s="27">
-        <f>(I59-I62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>179263.88529334666</v>
       </c>
       <c r="K59" s="27">
-        <f>(J59-J62)*(1+$B$22)</f>
+        <f t="shared" si="10"/>
         <v>182849.16299921359</v>
       </c>
       <c r="L59" s="16"/>
     </row>
-    <row r="60" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" s="11" customFormat="1">
       <c r="A60" s="26" t="s">
         <v>66</v>
       </c>
@@ -2176,7 +2179,7 @@
       <c r="J60" s="27"/>
       <c r="K60" s="27"/>
     </row>
-    <row r="61" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" s="11" customFormat="1">
       <c r="A61" s="26" t="s">
         <v>52</v>
       </c>
@@ -2191,7 +2194,7 @@
       <c r="J61" s="27"/>
       <c r="K61" s="28"/>
     </row>
-    <row r="62" spans="1:12" s="11" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" s="11" customFormat="1" ht="16.5" thickBot="1">
       <c r="A62" s="29" t="s">
         <v>34</v>
       </c>
@@ -2206,42 +2209,42 @@
       <c r="J62" s="30"/>
       <c r="K62" s="31"/>
     </row>
-    <row r="63" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" s="11" customFormat="1">
       <c r="B63" s="67"/>
       <c r="C63" s="68"/>
     </row>
-    <row r="64" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="72" t="s">
+    <row r="64" spans="1:12" s="11" customFormat="1"/>
+    <row r="65" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A65" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="72"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B65" s="81"/>
+      <c r="C65" s="81"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
+      <c r="F65" s="81"/>
+      <c r="G65" s="81"/>
+      <c r="H65" s="81"/>
+      <c r="I65" s="81"/>
+      <c r="J65" s="81"/>
+      <c r="K65" s="81"/>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="43"/>
-      <c r="B66" s="73" t="s">
+      <c r="B66" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
-      <c r="I66" s="74"/>
-      <c r="J66" s="74"/>
-      <c r="K66" s="75"/>
-    </row>
-    <row r="67" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="83"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="83"/>
+      <c r="H66" s="83"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="84"/>
+    </row>
+    <row r="67" spans="1:11" ht="16.5" thickBot="1">
       <c r="A67" s="44"/>
       <c r="B67" s="47">
         <v>1</v>
@@ -2274,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="57" t="s">
         <v>38</v>
       </c>
@@ -2289,7 +2292,7 @@
       <c r="J68" s="53"/>
       <c r="K68" s="53"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -2302,39 +2305,39 @@
         <v>37468.060066117148</v>
       </c>
       <c r="D69" s="6">
-        <f t="shared" ref="D69:K69" si="10">C69*(1+$B$21)</f>
+        <f t="shared" ref="D69:K69" si="11">C69*(1+$B$21)</f>
         <v>38217.421304907555</v>
       </c>
       <c r="E69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>38981.76976922313</v>
       </c>
       <c r="F69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>39761.405203589369</v>
       </c>
       <c r="G69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>40556.633347422568</v>
       </c>
       <c r="H69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>41367.766054927655</v>
       </c>
       <c r="I69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>42195.121417393981</v>
       </c>
       <c r="J69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>43039.023887936986</v>
       </c>
       <c r="K69" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>43899.804408734752</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -2347,39 +2350,39 @@
         <v>12000</v>
       </c>
       <c r="D70" s="6">
-        <f t="shared" ref="D70:K70" si="11">C70</f>
+        <f t="shared" ref="D70:K70" si="12">C70</f>
         <v>12000</v>
       </c>
       <c r="E70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="F70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="G70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="H70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="I70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="J70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
       <c r="K70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>-3061.1160154725289</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2401,348 +2404,335 @@
         <v>8044.4079161408226</v>
       </c>
       <c r="C72" s="6">
-        <f t="shared" ref="C72:K72" si="12">(C69)*(1+$B$22)^($B$25-C67+1)-(C69)</f>
+        <f t="shared" ref="C72:K72" si="13">(C69)*(1+$B$22)^($B$25-C67+1)-(C69)</f>
         <v>7309.7400795938229</v>
       </c>
       <c r="D72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6560.3788847032265</v>
       </c>
       <c r="E72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5796.0304642874544</v>
       </c>
       <c r="F72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5016.3950738210333</v>
       </c>
       <c r="G72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4221.1669738876444</v>
       </c>
       <c r="H72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3410.0343102823608</v>
       </c>
       <c r="I72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2582.6789917158458</v>
       </c>
       <c r="J72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1738.7765650726506</v>
       </c>
       <c r="K72" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>877.99608817469561</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B73" s="6"/>
-      <c r="D73" s="6"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D74" s="8"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B75" s="83"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="80"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+    <row r="74" spans="1:11">
+      <c r="B74" t="s">
         <v>8</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C74" t="s">
         <v>36</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="75" spans="1:11">
+      <c r="A75" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B75" s="6">
         <f>B69*((1+B22)*(-1+(1+B22))*((1+B22)^B25-(1+B21)^B25))/(B22*(-1+(1+B22)-B21))</f>
         <v>447778.04673245124</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C75" s="6">
         <f>B71*(1+B22)^B25-B71</f>
         <v>670.36732634506825</v>
       </c>
-      <c r="D79" s="6">
-        <f>C79+B79</f>
+      <c r="D75" s="6">
+        <f>C75+B75</f>
         <v>448448.4140587963</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="76" spans="1:11">
+      <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="82">
+      <c r="B76" s="76">
         <f>B69*(1-(1+B21)^10)/(1-(1+B21))</f>
         <v>402220.39764592296</v>
       </c>
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B81" s="6">
-        <f>B79-B80</f>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="B77" s="6">
+        <f>B75-B76</f>
         <v>45557.649086528283</v>
       </c>
-      <c r="C81" s="6"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="6">
-        <f>B79+C79-B80</f>
+      <c r="B79" s="6">
+        <f>B75+C75-B76</f>
         <v>46228.016412873345</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="6"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+    <row r="80" spans="1:11">
+      <c r="A80" s="6"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>76</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B82" s="4">
         <f>B69*(1+B22)*((1+B22)^B25-(1+B21)^B25)/(B22-B21)</f>
         <v>447778.03896473994</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C82" s="4">
         <f>B71*(1+B22)^B25</f>
         <v>3731.4833418175972</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="4">
+      <c r="B83" s="4">
         <f>B69*((1-(1+B21)^B25))/(1-(1+B21))</f>
         <v>402220.39764592296</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C83" s="6">
         <f>B71</f>
         <v>3061.1160154725289</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="84">
-        <f>B86-B87</f>
+      <c r="B84" s="77">
+        <f>B82-B83</f>
         <v>45557.641318816983</v>
       </c>
-      <c r="C88" s="6">
-        <f>C86-C87</f>
+      <c r="C84" s="6">
+        <f>C82-C83</f>
         <v>670.36732634506825</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
         <v>77</v>
       </c>
-      <c r="B90" s="6">
-        <f>B88+C88</f>
+      <c r="B86" s="6">
+        <f>B84+C84</f>
         <v>46228.008645162052</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="88" spans="1:3">
+      <c r="B88" t="s">
         <v>8</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C88" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="48"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+      <c r="B89" s="48"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B94" s="12"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="B90" s="12"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>88</v>
       </c>
-      <c r="B95" s="12">
+      <c r="B91" s="12">
         <f>B37*B25</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>89</v>
       </c>
-      <c r="B96" s="6"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B92" s="6"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="6">
-        <f>B95+B96</f>
+      <c r="B93" s="6">
+        <f>B91+B92</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+    <row r="94" spans="1:3">
+      <c r="A94" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>90</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B95" s="6">
         <f>B69*(1+B22)*((1+B22)^B25-(1+B21)^B25)/(B22-B21)</f>
         <v>447778.03896473994</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B100" s="80"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="B96" s="74"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>91</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B97" s="6">
         <f>B36*B35*(1+B22)^B25</f>
         <v>3731.4833418175972</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B98" s="6">
         <f>B35</f>
         <v>3061.1160154725289</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B103" s="48">
-        <f>B99-B100+B101-B102</f>
+      <c r="B99" s="48">
+        <f>B95-B96+B97-B98</f>
         <v>448448.406291085</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="12"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" s="72">
+        <f>B89+B93+B99+B101</f>
+        <v>568448.40629108506</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>81</v>
-      </c>
-      <c r="B105" s="12"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>94</v>
-      </c>
-      <c r="B107" s="78">
-        <f>B93+B97+B103+B105</f>
-        <v>568448.40629108506</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
         <v>97</v>
       </c>
-      <c r="B109" s="78">
+      <c r="B105" s="72">
         <f>B37*B25+B69*((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/(B22-B21)</f>
         <v>568448.40629108495</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
         <v>62</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B106" s="6">
         <f>B37*B25</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B107" s="6">
         <f>B69</f>
         <v>36733.392185670345</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
         <v>98</v>
       </c>
-      <c r="B112" s="85">
+      <c r="B108" s="78">
         <f>((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)</f>
         <v>-1.2208194761549431E-8</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B113" s="6">
-        <f>B110+B111*B112</f>
+    <row r="109" spans="1:2">
+      <c r="B109" s="6">
+        <f>B106+B107*B108</f>
         <v>119999.99955155159</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="78">
-        <f>(G37-B110)*(B22-B21)</f>
+      <c r="B113" s="72">
+        <f>(G37-B106)*(B22-B21)</f>
         <v>-4.4844840605504148E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
         <v>100</v>
       </c>
-      <c r="B118" s="81">
+      <c r="B114" s="75">
         <f>((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)</f>
         <v>-1.2208194761549431E-8</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
         <v>99</v>
       </c>
-      <c r="B120" s="6">
-        <f>(G37-B110)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
+      <c r="B116" s="6">
+        <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
         <v>3061.1160154725289</v>
       </c>
     </row>
@@ -2762,32 +2752,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E10B24D-E85D-FF45-A47C-BC8222E46AB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.375" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
     <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="71"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="80"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="70"/>
       <c r="B2" s="70"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="70" t="s">
         <v>61</v>
       </c>
@@ -2795,7 +2785,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="70"/>
       <c r="B4" s="70"/>
       <c r="E4" s="3" t="s">
@@ -2805,7 +2795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2817,7 +2807,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2832,7 +2822,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2843,7 +2833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2858,17 +2848,17 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="80"/>
       <c r="E10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2883,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2894,12 +2884,12 @@
       <c r="E12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="72">
         <f>B6*B28*B25</f>
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
         <v>65</v>
       </c>
@@ -2909,24 +2899,24 @@
       <c r="E13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="78">
+      <c r="F13" s="72">
         <f>(B29)*B25</f>
         <v>240000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="78">
+      <c r="F14" s="72">
         <f>B31*B25</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -2936,12 +2926,12 @@
       <c r="E15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="78">
+      <c r="F15" s="72">
         <f>B30*B25</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -2952,12 +2942,12 @@
       <c r="E16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="78">
+      <c r="F16" s="72">
         <f>SUM(F11:F15)</f>
         <v>580000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
@@ -2965,18 +2955,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="80"/>
       <c r="E19" t="s">
         <v>33</v>
       </c>
@@ -2985,7 +2975,7 @@
         <v>72036.642737751681</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -3000,7 +2990,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3009,7 +2999,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3021,7 +3011,7 @@
       </c>
       <c r="F22" s="48"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3029,7 +3019,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3040,7 +3030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -3052,11 +3042,11 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="71" t="s">
+    <row r="26" spans="1:6">
+      <c r="A26" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="71"/>
+      <c r="B26" s="80"/>
       <c r="E26" t="s">
         <v>43</v>
       </c>
@@ -3065,7 +3055,7 @@
         <v>480244.28491834458</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -3080,7 +3070,7 @@
         <v>380244.28491834458</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -3095,7 +3085,7 @@
         <v>83653.742682035794</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -3107,7 +3097,7 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -3117,12 +3107,12 @@
       <c r="E30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="77">
+      <c r="F30" s="71">
         <f>F26-F28</f>
         <v>396590.5422363088</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -3130,35 +3120,35 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="E32" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F32" s="49"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="18">
       <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="79">
+      <c r="B34" s="73">
         <f>F34/((1-(1+B21)^B25)/(1-(1+B21)))/12</f>
         <v>3085.6653829440797</v>
       </c>
       <c r="E34" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="78">
+      <c r="F34" s="72">
         <f>F8+F16+F19-F30</f>
         <v>405446.10050144291</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>56</v>
       </c>

</xml_diff>